<commit_message>
Update Analisi_Previsioni_SRKT2.xlsx and remove temporary file
</commit_message>
<xml_diff>
--- a/.revised/Analisi_Previsioni_SRKT2.xlsx
+++ b/.revised/Analisi_Previsioni_SRKT2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Websites\faco-dmek-revised\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Websites\faco-dmek-improved\.revised\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D63DC0-4D85-4497-8BBB-2FE3AB24BA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483E1AEB-F1AA-44F0-980B-4FB1CE1DC6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:XFD96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>